<commit_message>
Rename Headings to Features
</commit_message>
<xml_diff>
--- a/data_impute_project/corr_combinations/bird/combination_1_ABCD_correlation_results.xlsx
+++ b/data_impute_project/corr_combinations/bird/combination_1_ABCD_correlation_results.xlsx
@@ -436,12 +436,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Variable 1</t>
+          <t>Feature 1</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Variable 2</t>
+          <t>Feature 2</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">

</xml_diff>